<commit_message>
Report History update 1
Report History update 1
</commit_message>
<xml_diff>
--- a/sampleData.xlsx
+++ b/sampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveswinburneeduau-my.sharepoint.com/personal/101100655_student_swin_edu_au/Documents/2020 - Semester 2/DP2/Project/GitHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/89834c650c126c85/Documents/GitHub/DP2_pass/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3" documentId="8_{CB8EF88B-26E2-4CE6-938E-2D478B36A621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FA26D92-9715-40C8-B2DD-A67A37EBCF9F}"/>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>